<commit_message>
Ajustes a datos formulario
</commit_message>
<xml_diff>
--- a/Maquinas Virtuales/CarteraInsolvenciaProcesoAdminfo/Configuraciones/Config_pruebas.xlsx
+++ b/Maquinas Virtuales/CarteraInsolvenciaProcesoAdminfo/Configuraciones/Config_pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacostri\Downloads\DesarrollosRPA-EPM-master\DesarrollosRPA-EPM-master\Maquinas Virtuales\CarteraInsolvenciaProcesoAdminfo\Configuraciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE9EE05-BF5E-4696-BED4-E0F85D3453A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4D385E-565D-44CD-B290-C74E16CD6C30}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -229,6 +229,18 @@
   </si>
   <si>
     <t>C:\Users\jacostri\Desktop\PruebasAdminfo.xlsx</t>
+  </si>
+  <si>
+    <t>tecnologoEPM</t>
+  </si>
+  <si>
+    <t>observaciones</t>
+  </si>
+  <si>
+    <t>Gestionado por Jose Luis Rivera</t>
+  </si>
+  <si>
+    <t>Jose Ramiro Cardona</t>
   </si>
 </sst>
 </file>
@@ -591,7 +603,7 @@
   <dimension ref="A1:Z980"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -729,8 +741,22 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Se realiza homologacion de ambiente
</commit_message>
<xml_diff>
--- a/Maquinas Virtuales/CarteraInsolvenciaProcesoAdminfo/Configuraciones/Config_pruebas.xlsx
+++ b/Maquinas Virtuales/CarteraInsolvenciaProcesoAdminfo/Configuraciones/Config_pruebas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacostri\Downloads\DesarrollosRPA-EPM-master\DesarrollosRPA-EPM-master\Maquinas Virtuales\CarteraInsolvenciaProcesoAdminfo\Configuraciones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thanos\Desktop\CarteraInsolvenciaProcesoAdminfo\Configuraciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4D385E-565D-44CD-B290-C74E16CD6C30}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -168,15 +167,9 @@
     <t>RutaDatos</t>
   </si>
   <si>
-    <t>CredencialServidorCorreoExchange</t>
-  </si>
-  <si>
     <t>Credential</t>
   </si>
   <si>
-    <t>CredencialServidorCorreoExchange.Pruebas</t>
-  </si>
-  <si>
     <t>CorreoServidorExchange</t>
   </si>
   <si>
@@ -228,9 +221,6 @@
     <t>CredencialUsuarioAdminfo.Pruebas</t>
   </si>
   <si>
-    <t>C:\Users\jacostri\Desktop\PruebasAdminfo.xlsx</t>
-  </si>
-  <si>
     <t>tecnologoEPM</t>
   </si>
   <si>
@@ -241,12 +231,27 @@
   </si>
   <si>
     <t>Jose Ramiro Cardona</t>
+  </si>
+  <si>
+    <t>C:\Users\thanos\Desktop\CarteraInsolvenciaProcesoAdminfo\PruebasAdminfo</t>
+  </si>
+  <si>
+    <t>C:\Users\thanos\Desktop\CarteraInsolvenciaProcesoAdminfo\PruebasAdminfo.xlsx</t>
+  </si>
+  <si>
+    <t>CredencialesCorreo</t>
+  </si>
+  <si>
+    <t>CredencialServidorCorreoExchangeAdminfo</t>
+  </si>
+  <si>
+    <t>CredencialServidorCorreoExchangeAdminfo.Pruebas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -599,11 +604,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z980"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -664,101 +669,112 @@
         <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" t="s">
         <v>69</v>
-      </c>
-      <c r="B11" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>70</v>
       </c>
-      <c r="B12" t="s">
-        <v>71</v>
-      </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1727,7 +1743,7 @@
     <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" xr:uid="{CDDAB9AB-0726-40BD-9D4C-F7F3968567BC}"/>
+    <hyperlink ref="B9" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1735,7 +1751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2949,11 +2965,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2999,24 +3015,24 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" t="s">
         <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>